<commit_message>
Adding new Excel file as map
</commit_message>
<xml_diff>
--- a/JSon/megye_pbi.xlsx
+++ b/JSon/megye_pbi.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\Projects\TIMEA_Quarto_ShinyLive_Megye_R\JSon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6E1BF89B-E4B0-4973-B8E5-90E8A801C778}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E610C05F-7D5C-4346-8D16-542B14E10295}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="megye_pbi" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -164,12 +164,75 @@
   </si>
   <si>
     <t>Veszprém</t>
+  </si>
+  <si>
+    <t>OBJECTID_1</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -665,8 +728,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1021,570 +1085,638 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>135683.00889999999</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>135683.00889999999</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>135683.00889999999</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>525120416.30000001</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>459890.96240000002</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>459890.96240000002</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>459890.96240000002</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>4429748819</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>605010.54960000003</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>605010.54960000003</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
         <v>36</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>605010.54960000003</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>8443082626</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
         <v>485953.69890000002</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>485953.69890000002</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
         <v>37</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>485953.69890000002</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>5629672994</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>701855.4632</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>701855.4632</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>701855.4632</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>7246960995</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
         <v>388624.25589999999</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>388624.25589999999</v>
       </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>388624.25589999999</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>4261750812</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
         <v>408058.6458</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>408058.6458</v>
       </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
         <v>40</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>408058.6458</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>4358035429</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
         <v>524935.47210000001</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>524935.47210000001</v>
       </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
         <v>41</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>524935.47210000001</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>4208102507</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
         <v>479025.4486</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>479025.4486</v>
       </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>479025.4486</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>6208525517</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
         <v>428256.59889999998</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>428256.59889999998</v>
       </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
         <v>19</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>428256.59889999998</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>3637131206</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
         <v>322450.46159999998</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>322450.46159999998</v>
       </c>
-      <c r="D12">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>322450.46159999998</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>2263978152</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
         <v>384402.10369999998</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>384402.10369999998</v>
       </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
         <v>44</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>384402.10369999998</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>2544226293</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
         <v>691312.79639999999</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>691312.79639999999</v>
       </c>
-      <c r="D14">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
         <v>23</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>691312.79639999999</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>6390326245</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
         <v>577661.90870000003</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>577661.90870000003</v>
       </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
         <v>25</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>577661.90870000003</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>6064720659</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
         <v>565271.04330000002</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>565271.04330000002</v>
       </c>
-      <c r="D16">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
         <v>45</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>565271.04330000002</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>5933222282</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
         <v>518289.03259999998</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>518289.03259999998</v>
       </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" t="s">
         <v>46</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>518289.03259999998</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>5581363278</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
         <v>462074.83809999999</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>462074.83809999999</v>
       </c>
-      <c r="D18">
+      <c r="F18" s="1">
         <v>17</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>29</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>462074.83809999999</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>3702972865</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
         <v>491600.3284</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>491600.3284</v>
       </c>
-      <c r="D19">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>491600.3284</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>3336015074</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
         <v>424654.73670000001</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>424654.73670000001</v>
       </c>
-      <c r="D20">
-        <v>19</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" t="s">
         <v>47</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>424654.73670000001</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>4462965368</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
         <v>374818.70400000003</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <v>374818.70400000003</v>
       </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
         <v>34</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>374818.70400000003</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>3783502874</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>